<commit_message>
Add support for exporting data and caching zipcode-to-geolocation map
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Work/github/shmmsra/map-plotter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898CF5D-7478-6448-9ECC-F8D148B85971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676B54F9-1225-6342-9AE8-C91D1CA39726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Exeter Office Postcode</t>
   </si>
   <si>
-    <t>Lancing Offcie Postcode</t>
-  </si>
-  <si>
     <t>Leeds Office Postcode</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>07660</t>
+  </si>
+  <si>
+    <t>Lancing Office Postcode</t>
   </si>
 </sst>
 </file>
@@ -203,11 +203,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -465,7 +467,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD8"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -521,37 +523,37 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -559,49 +561,49 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q2" s="2">
         <v>53224</v>
@@ -613,10 +615,10 @@
         <v>10005</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -624,49 +626,49 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q3" s="2">
         <v>53224</v>
@@ -678,10 +680,10 @@
         <v>10005</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -689,49 +691,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="E4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q4" s="2">
         <v>53224</v>
@@ -743,10 +745,10 @@
         <v>10005</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -754,49 +756,49 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q5" s="2">
         <v>53224</v>
@@ -808,10 +810,10 @@
         <v>10005</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -819,49 +821,49 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q6" s="2">
         <v>53224</v>
@@ -873,10 +875,10 @@
         <v>10005</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -884,49 +886,49 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q7" s="2">
         <v>53224</v>
@@ -938,10 +940,10 @@
         <v>10005</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -949,49 +951,49 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="Q8" s="2">
         <v>53224</v>
@@ -1003,13 +1005,14 @@
         <v>10005</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor Google Map API key storage location
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Work/github/shmmsra/map-plotter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA928F3-5BD4-334F-9955-971C89ECE25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E03DE88-985C-6848-B44B-8D0B243B6FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3633" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3633" uniqueCount="57">
   <si>
     <t>Employee ID</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Lancing Office Postcode</t>
+  </si>
+  <si>
+    <t>Supriya Tiwari</t>
+  </si>
+  <si>
+    <t>YO612PS</t>
   </si>
 </sst>
 </file>
@@ -466,8 +472,8 @@
   </sheetPr>
   <dimension ref="A1:U225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A225"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -491,7 +497,7 @@
     <col min="21" max="21" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +562,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -621,7 +627,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -686,7 +692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -751,7 +757,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -816,7 +822,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -881,7 +887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -946,7 +952,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1019,10 +1025,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>23</v>

</xml_diff>